<commit_message>
Commit Message Change Test Suite Setup and Teardown
</commit_message>
<xml_diff>
--- a/TestCases/InputData.xlsx
+++ b/TestCases/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>${Invitation_Code}</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Abcdefg_1</t>
-  </si>
-  <si>
-    <t>0693</t>
   </si>
   <si>
     <t>${CVNNumber}</t>
@@ -598,7 +595,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>1114173323</v>
@@ -626,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,10 +648,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1111111113</v>
+        <v>1005254554</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -719,82 +716,82 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
@@ -808,37 +805,37 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="F2" s="3">
         <v>1425789658974510</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="O2" s="1">
         <v>11554</v>
@@ -850,7 +847,7 @@
         <v>323256348</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S2" s="3">
         <v>874598745874</v>
@@ -859,31 +856,31 @@
         <v>741258963</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -919,10 +916,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -930,7 +927,7 @@
         <v>1005254554</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -976,13 +973,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1014,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1040,16 +1037,16 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1057,7 +1054,7 @@
         <v>1005254554</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1072,7 +1069,7 @@
         <v>44742</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>